<commit_message>
added changes to sop
</commit_message>
<xml_diff>
--- a/TADA/PT_math.xlsx
+++ b/TADA/PT_math.xlsx
@@ -79,15 +79,9 @@
     <t>Intercept</t>
   </si>
   <si>
-    <t>amps</t>
-  </si>
-  <si>
     <t>Enter</t>
   </si>
   <si>
-    <t>bits</t>
-  </si>
-  <si>
     <t>Voltage</t>
   </si>
   <si>
@@ -100,9 +94,6 @@
     <t>Resistance</t>
   </si>
   <si>
-    <t>ohms</t>
-  </si>
-  <si>
     <t>psi</t>
   </si>
   <si>
@@ -116,6 +107,15 @@
   </si>
   <si>
     <t>sse</t>
+  </si>
+  <si>
+    <t>units</t>
+  </si>
+  <si>
+    <t>ohm</t>
+  </si>
+  <si>
+    <t>amp</t>
   </si>
 </sst>
 </file>
@@ -153,7 +153,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -165,17 +165,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -191,13 +180,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -209,15 +191,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -231,16 +204,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -273,44 +244,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US"/>
-              <a:t>Calibration</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Line Fit</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:layout>
-        <c:manualLayout>
-          <c:xMode val="edge"/>
-          <c:yMode val="edge"/>
-          <c:x val="0.35019444444444442"/>
-          <c:y val="2.7777777777777776E-2"/>
-        </c:manualLayout>
-      </c:layout>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -351,17 +285,17 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$4</c:f>
+              <c:f>Sheet1!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>mA</c:v>
+                  <c:v>PSI</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -396,12 +330,7 @@
             <c:dispRSqr val="1"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
-              <c:layout>
-                <c:manualLayout>
-                  <c:x val="-1.890944881889764E-2"/>
-                  <c:y val="-3.865886555847186E-2"/>
-                </c:manualLayout>
-              </c:layout>
+              <c:layout/>
               <c:numFmt formatCode="General" sourceLinked="0"/>
               <c:spPr>
                 <a:noFill/>
@@ -434,6 +363,30 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Sheet1!$A$5:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>4.0129999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.021000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>20.027999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>12.023</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.0119999999999996</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Sheet1!$B$5:$B$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -455,30 +408,6 @@
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Sheet1!$C$5:$C$9</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4.0129999999999999</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>12.021000000000001</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>20.027999999999999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>12.023</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4.0119999999999996</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
@@ -490,11 +419,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="229041728"/>
-        <c:axId val="229048800"/>
+        <c:axId val="1078899024"/>
+        <c:axId val="1078904464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="229041728"/>
+        <c:axId val="1078899024"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -514,62 +443,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>PSI</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -607,12 +480,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229048800"/>
+        <c:crossAx val="1078904464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="229048800"/>
+        <c:axId val="1078904464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -632,62 +505,6 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>mA</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -725,7 +542,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="229041728"/>
+        <c:crossAx val="1078899024"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1335,19 +1152,19 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>185737</xdr:rowOff>
+      <xdr:colOff>328612</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>23812</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>71437</xdr:rowOff>
+      <xdr:rowOff>80962</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -1630,13 +1447,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:H28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1645,28 +1463,28 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>2</v>
-      </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="E4" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B5" s="4">
+      <c r="A5" s="5">
+        <v>4.0129999999999999</v>
+      </c>
+      <c r="B5" s="5">
         <v>0</v>
       </c>
-      <c r="C5" s="5">
-        <v>4.0129999999999999</v>
-      </c>
       <c r="D5">
-        <f>$C$13*C5+$C$14</f>
+        <f>$C$13*A5+$C$14</f>
         <v>4.5116128785549492E-5</v>
       </c>
       <c r="E5">
@@ -1675,66 +1493,66 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
+      <c r="A6" s="5">
+        <v>12.021000000000001</v>
+      </c>
+      <c r="B6" s="5">
         <v>2.5</v>
       </c>
-      <c r="C6" s="5">
-        <v>12.021000000000001</v>
-      </c>
       <c r="D6">
-        <f t="shared" ref="D6:D9" si="0">$C$13*C6+$C$14</f>
+        <f>$C$13*A6+$C$14</f>
         <v>2.5000080729471765</v>
       </c>
       <c r="E6">
-        <f t="shared" ref="E6:E9" si="1">(B6-D6)^2</f>
+        <f t="shared" ref="E6:E9" si="0">(B6-D6)^2</f>
         <v>6.5172476115035789E-11</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="4">
+      <c r="A7" s="5">
+        <v>20.027999999999999</v>
+      </c>
+      <c r="B7" s="5">
         <v>5</v>
       </c>
-      <c r="C7" s="5">
-        <v>20.027999999999999</v>
-      </c>
       <c r="D7">
+        <f>$C$13*A7+$C$14</f>
+        <v>4.9996588465791518</v>
+      </c>
+      <c r="E7">
         <f t="shared" si="0"/>
-        <v>4.9996588465791518</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="1"/>
         <v>1.1638565655641035E-7</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="A8" s="5">
+        <v>12.023</v>
+      </c>
+      <c r="B8" s="5">
         <v>2.5</v>
       </c>
-      <c r="C8" s="5">
-        <v>12.023</v>
-      </c>
       <c r="D8">
+        <f>$C$13*A8+$C$14</f>
+        <v>2.5006324393200083</v>
+      </c>
+      <c r="E8">
         <f t="shared" si="0"/>
-        <v>2.5006324393200083</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="1"/>
         <v>3.9997949349260871E-7</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6">
+        <v>4.0119999999999996</v>
+      </c>
       <c r="B9" s="6">
         <v>0</v>
       </c>
-      <c r="C9" s="7">
-        <v>4.0119999999999996</v>
-      </c>
       <c r="D9">
+        <f>$C$13*A9+$C$14</f>
+        <v>-2.670670576305767E-4</v>
+      </c>
+      <c r="E9">
         <f t="shared" si="0"/>
-        <v>-2.670670576305767E-4</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="1"/>
         <v>7.1324813271453779E-8</v>
       </c>
     </row>
@@ -1766,32 +1584,32 @@
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="8">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2">
         <v>1023</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>10</v>
+      <c r="C20" s="2" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B21">
         <f>(B20+1)/204.8</f>
         <v>5</v>
       </c>
       <c r="C21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H21" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -1799,18 +1617,18 @@
         <v>3</v>
       </c>
       <c r="F23" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B24">
         <v>263</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -1822,7 +1640,7 @@
         <v>1.9011406844106463E-2</v>
       </c>
       <c r="C25" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -1835,15 +1653,15 @@
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
+      <c r="A28" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="8">
-        <f>(B26-C14)/C13</f>
-        <v>64.911096230753415</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>16</v>
+      <c r="B28" s="2">
+        <f>C13*B26+C14</f>
+        <v>4.6822955558837291</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>